<commit_message>
add group support: not complete
</commit_message>
<xml_diff>
--- a/packages/wasm/src/snapshots/imexport_wasm__tests__tests__create_template_should_be_correct.snap.xlsx
+++ b/packages/wasm/src/snapshots/imexport_wasm__tests__tests__create_template_should_be_correct.snap.xlsx
@@ -14,22 +14,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <si>
+    <t>Tom and Jerry</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Generations</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>Category</t>
+    <t>Birth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,13 +46,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -58,8 +88,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,24 +390,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="50" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update parent column feature
</commit_message>
<xml_diff>
--- a/packages/wasm/src/snapshots/imexport_wasm__tests__tests__create_template_should_be_correct.snap.xlsx
+++ b/packages/wasm/src/snapshots/imexport_wasm__tests__tests__create_template_should_be_correct.snap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tom and Jerry</t>
   </si>
@@ -22,10 +22,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Generations</t>
+    <t>Life</t>
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Generation</t>
   </si>
   <si>
     <t>Age</t>
@@ -390,13 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="50" customHeight="1">
@@ -411,31 +416,39 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
+    <row r="4" spans="1:4" ht="30" customHeight="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add columns parent check and the order check
</commit_message>
<xml_diff>
--- a/packages/wasm/src/snapshots/imexport_wasm__tests__tests__create_template_should_be_correct.snap.xlsx
+++ b/packages/wasm/src/snapshots/imexport_wasm__tests__tests__create_template_should_be_correct.snap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Tom and Jerry</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Generation</t>
+  </si>
+  <si>
+    <t>Heart</t>
   </si>
   <si>
     <t>Age</t>
@@ -393,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,18 +404,19 @@
   <cols>
     <col min="1" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="50" customHeight="1">
+    <row r="1" spans="1:5" ht="50" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1">
+    <row r="2" spans="1:5" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -420,35 +424,41 @@
         <v>2</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1">
+    <row r="3" spans="1:5" ht="30" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1">
+    <row r="4" spans="1:5" ht="30" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E2:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>